<commit_message>
trying to make file comparison more robust
</commit_message>
<xml_diff>
--- a/feedback_forms/current_versions/dairy_digester_operator_feedback_v006.xlsx
+++ b/feedback_forms/current_versions/dairy_digester_operator_feedback_v006.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://carb.sharepoint.com/teams/RDSatelliteProject/Shared Documents/General/RD-ED-ISD High-level Planning/Operator Notification Materials for Review/spreadsheets/xl_workbooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tony_local\pycharm\feedback_portal\feedback_forms\current_versions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{BAD62B58-6BA2-4454-B1E3-BB434B98D284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA90B523-98E9-4008-B6DD-978E7FFEB112}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8411910C-B1AE-464A-BDF4-716FFD82F86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3347" yWindow="773" windowWidth="19200" windowHeight="11387" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
+    <workbookView xWindow="3687" yWindow="1113" windowWidth="19200" windowHeight="11387" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedback Form" sheetId="6" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="338">
   <si>
     <t>CARB Methane Plume Detection</t>
   </si>
@@ -1512,18 +1512,12 @@
     <t>jinja_contact_email</t>
   </si>
   <si>
-    <t>me@email.com</t>
-  </si>
-  <si>
     <t>$D$33</t>
   </si>
   <si>
     <t>jinja_contact_name</t>
   </si>
   <si>
-    <t>Contact Person Name</t>
-  </si>
-  <si>
     <t>$D$34</t>
   </si>
   <si>
@@ -1636,9 +1630,6 @@
   </si>
   <si>
     <t>jinja_manure_anaerobic_lagoon</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>$D$66</t>
@@ -2107,7 +2098,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2147,7 +2138,6 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2196,104 +2186,95 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -3656,405 +3637,405 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="4.1171875" style="66" customWidth="1"/>
-    <col min="2" max="2" width="65.703125" style="66" customWidth="1"/>
-    <col min="3" max="3" width="4.703125" style="66" customWidth="1"/>
-    <col min="4" max="4" width="65.703125" style="66" customWidth="1"/>
-    <col min="5" max="5" width="4.1171875" style="66" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="66"/>
+    <col min="1" max="1" width="4.1171875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="65.703125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="4.703125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="65.703125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="4.1171875" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="34" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-    </row>
-    <row r="2" spans="2:5" s="34" customFormat="1" ht="51" x14ac:dyDescent="0.5">
-      <c r="B2" s="35" t="s">
+    <row r="1" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="2:5" s="33" customFormat="1" ht="51" x14ac:dyDescent="0.5">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-    </row>
-    <row r="3" spans="2:5" s="34" customFormat="1" ht="51" x14ac:dyDescent="0.5">
-      <c r="B3" s="36" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+    </row>
+    <row r="3" spans="2:5" s="33" customFormat="1" ht="51" x14ac:dyDescent="0.5">
+      <c r="B3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-    </row>
-    <row r="4" spans="2:5" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="38"/>
-    </row>
-    <row r="5" spans="2:5" s="34" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-    </row>
-    <row r="6" spans="2:5" s="41" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="40"/>
-    </row>
-    <row r="7" spans="2:5" s="34" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="8" spans="2:5" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B8" s="42" t="s">
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+    </row>
+    <row r="4" spans="2:5" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="37"/>
+    </row>
+    <row r="5" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+    </row>
+    <row r="6" spans="2:5" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="39"/>
+    </row>
+    <row r="7" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B8" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-    </row>
-    <row r="9" spans="2:5" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B9" s="45" t="s">
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+    </row>
+    <row r="9" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B9" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="43"/>
-    </row>
-    <row r="10" spans="2:5" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B10" s="47" t="s">
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="42"/>
+    </row>
+    <row r="10" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B10" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="43"/>
-    </row>
-    <row r="11" spans="2:5" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B11" s="42" t="s">
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="42"/>
+    </row>
+    <row r="11" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B11" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-    </row>
-    <row r="12" spans="2:5" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B12" s="42" t="s">
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+    </row>
+    <row r="12" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-    </row>
-    <row r="13" spans="2:5" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B13" s="42" t="s">
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+    </row>
+    <row r="13" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B13" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-    </row>
-    <row r="14" spans="2:5" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B14" s="42" t="s">
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+    </row>
+    <row r="14" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B14" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-    </row>
-    <row r="15" spans="2:5" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B15" s="49" t="s">
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+    </row>
+    <row r="15" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B15" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-    </row>
-    <row r="16" spans="2:5" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B16" s="42" t="s">
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+    </row>
+    <row r="16" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B16" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-    </row>
-    <row r="17" spans="2:5" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B17" s="42" t="s">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+    </row>
+    <row r="17" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B17" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-    </row>
-    <row r="18" spans="2:5" s="34" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="19" spans="2:5" s="41" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="40"/>
-    </row>
-    <row r="20" spans="2:5" s="34" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="21" spans="2:5" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B21" s="42" t="s">
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+    </row>
+    <row r="18" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="19" spans="2:5" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="39"/>
+    </row>
+    <row r="20" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="21" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B21" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="51">
+      <c r="C21" s="42"/>
+      <c r="D21" s="50">
         <v>153</v>
       </c>
-      <c r="E21" s="42"/>
-    </row>
-    <row r="22" spans="2:5" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B22" s="42" t="s">
+      <c r="E21" s="41"/>
+    </row>
+    <row r="22" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B22" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="43"/>
-      <c r="D22" s="51">
+      <c r="C22" s="42"/>
+      <c r="D22" s="50">
         <v>7143</v>
       </c>
-      <c r="E22" s="43"/>
-    </row>
-    <row r="23" spans="2:5" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B23" s="42" t="s">
+      <c r="E22" s="42"/>
+    </row>
+    <row r="23" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B23" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="53">
+      <c r="C23" s="42"/>
+      <c r="D23" s="51">
         <v>45782.517916666664</v>
       </c>
-      <c r="E23" s="43"/>
-    </row>
-    <row r="24" spans="2:5" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B24" s="42" t="s">
+      <c r="E23" s="42"/>
+    </row>
+    <row r="24" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B24" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="51">
+      <c r="C24" s="42"/>
+      <c r="D24" s="50">
         <v>36.076599999999999</v>
       </c>
-      <c r="E24" s="42"/>
-    </row>
-    <row r="25" spans="2:5" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B25" s="42" t="s">
+      <c r="E24" s="41"/>
+    </row>
+    <row r="25" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B25" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="43"/>
-      <c r="D25" s="51">
+      <c r="C25" s="42"/>
+      <c r="D25" s="50">
         <v>-119.44289999999999</v>
       </c>
-      <c r="E25" s="42"/>
-    </row>
-    <row r="26" spans="2:5" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B26" s="42" t="s">
+      <c r="E25" s="41"/>
+    </row>
+    <row r="26" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B26" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="43"/>
-      <c r="D26" s="53" t="s">
+      <c r="C26" s="42"/>
+      <c r="D26" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="42"/>
-    </row>
-    <row r="27" spans="2:5" s="34" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="28" spans="2:5" s="41" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="40"/>
-    </row>
-    <row r="29" spans="2:5" s="34" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="30" spans="2:5" s="34" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="B30" s="54" t="s">
+      <c r="E26" s="41"/>
+    </row>
+    <row r="27" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="28" spans="2:5" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="39"/>
+    </row>
+    <row r="29" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="30" spans="2:5" s="33" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+      <c r="B30" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:5" s="34" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="B31" s="54" t="s">
+    <row r="31" spans="2:5" s="33" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+      <c r="B31" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="32" t="s">
+      <c r="D31" s="31" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="2:5" s="34" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="B32" s="54" t="s">
+    <row r="32" spans="2:5" s="33" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+      <c r="B32" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="32" t="s">
+      <c r="D32" s="31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="2:5" s="52" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="B33" s="55" t="s">
+    <row r="33" spans="2:5" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+      <c r="B33" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="55"/>
-      <c r="D33" s="30" t="s">
+      <c r="C33" s="53"/>
+      <c r="D33" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E33" s="56"/>
-    </row>
-    <row r="34" spans="2:5" s="52" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="B34" s="55" t="s">
+      <c r="E33" s="54"/>
+    </row>
+    <row r="34" spans="2:5" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+      <c r="B34" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="55"/>
-      <c r="D34" s="30" t="s">
+      <c r="C34" s="53"/>
+      <c r="D34" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E34" s="56"/>
-    </row>
-    <row r="35" spans="2:5" s="52" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="B35" s="55" t="s">
+      <c r="E34" s="54"/>
+    </row>
+    <row r="35" spans="2:5" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+      <c r="B35" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="55"/>
-      <c r="D35" s="30" t="s">
+      <c r="C35" s="53"/>
+      <c r="D35" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="56"/>
-    </row>
-    <row r="36" spans="2:5" s="34" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="37" spans="2:5" s="41" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B37" s="39"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="40"/>
-    </row>
-    <row r="38" spans="2:5" s="34" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="39" spans="2:5" s="52" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
-      <c r="B39" s="55" t="s">
+      <c r="E35" s="54"/>
+    </row>
+    <row r="36" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="37" spans="2:5" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="39"/>
+    </row>
+    <row r="38" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="39" spans="2:5" s="10" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
+      <c r="B39" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="55"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="57"/>
-    </row>
-    <row r="40" spans="2:5" s="52" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
-      <c r="B40" s="58" t="s">
+      <c r="C39" s="53"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="55"/>
+    </row>
+    <row r="40" spans="2:5" s="10" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
+      <c r="B40" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="56"/>
-      <c r="D40" s="30"/>
-    </row>
-    <row r="41" spans="2:5" s="34" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
-      <c r="B41" s="58" t="s">
+      <c r="C40" s="54"/>
+      <c r="D40" s="29"/>
+    </row>
+    <row r="41" spans="2:5" s="33" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
+      <c r="B41" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="D41" s="30"/>
-    </row>
-    <row r="42" spans="2:5" s="52" customFormat="1" ht="30.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B42" s="54" t="s">
+      <c r="D41" s="29"/>
+    </row>
+    <row r="42" spans="2:5" s="10" customFormat="1" ht="30.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="56"/>
-      <c r="D42" s="30" t="s">
+      <c r="C42" s="54"/>
+      <c r="D42" s="29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="2:5" s="52" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B43" s="58" t="s">
+    <row r="43" spans="2:5" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B43" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="56"/>
-      <c r="D43" s="19" t="s">
+      <c r="C43" s="54"/>
+      <c r="D43" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="2:5" s="52" customFormat="1" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B44" s="58" t="s">
+    <row r="44" spans="2:5" s="10" customFormat="1" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B44" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="56"/>
-      <c r="D44" s="19" t="s">
+      <c r="C44" s="54"/>
+      <c r="D44" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="2:5" s="52" customFormat="1" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B45" s="58" t="s">
+    <row r="45" spans="2:5" s="10" customFormat="1" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B45" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="C45" s="56"/>
-      <c r="D45" s="31" t="s">
+      <c r="C45" s="54"/>
+      <c r="D45" s="30" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="2:5" s="52" customFormat="1" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B46" s="55" t="s">
+    <row r="46" spans="2:5" s="10" customFormat="1" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="56"/>
-      <c r="D46" s="19" t="s">
+      <c r="C46" s="54"/>
+      <c r="D46" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="2:5" s="52" customFormat="1" ht="45.7" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="B47" s="59" t="s">
+    <row r="47" spans="2:5" s="10" customFormat="1" ht="45.7" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="B47" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D47" s="31" t="s">
+      <c r="D47" s="30" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="2:5" s="34" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="49" spans="2:5" s="41" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B49" s="39"/>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="40"/>
-    </row>
-    <row r="50" spans="2:5" s="34" customFormat="1" ht="15.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B50" s="55"/>
-    </row>
-    <row r="51" spans="2:5" s="52" customFormat="1" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B51" s="55" t="s">
+    <row r="48" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="49" spans="2:5" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="39"/>
+    </row>
+    <row r="50" spans="2:5" s="33" customFormat="1" ht="15.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B50" s="53"/>
+    </row>
+    <row r="51" spans="2:5" s="10" customFormat="1" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B51" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C51" s="56"/>
-      <c r="D51" s="19" t="s">
+      <c r="C51" s="54"/>
+      <c r="D51" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="2:5" s="52" customFormat="1" ht="15.7" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="B52" s="55" t="s">
+    <row r="52" spans="2:5" s="10" customFormat="1" ht="15.7" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="B52" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="D52" s="31" t="s">
+      <c r="D52" s="30" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="2:5" s="52" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
-      <c r="B53" s="55" t="s">
+    <row r="53" spans="2:5" s="10" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
+      <c r="B53" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="D53" s="30" t="s">
+      <c r="D53" s="29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="2:5" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B54" s="56"/>
-      <c r="C54" s="56"/>
-      <c r="D54" s="56"/>
-    </row>
-    <row r="55" spans="2:5" s="41" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B55" s="39"/>
-      <c r="C55" s="39"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="40"/>
-    </row>
-    <row r="56" spans="2:5" s="34" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="57" spans="2:5" s="52" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
-      <c r="B57" s="58" t="s">
+    <row r="54" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B54" s="54"/>
+      <c r="C54" s="54"/>
+      <c r="D54" s="54"/>
+    </row>
+    <row r="55" spans="2:5" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B55" s="38"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="39"/>
+    </row>
+    <row r="56" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="57" spans="2:5" s="10" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
+      <c r="B57" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="C57" s="56"/>
-      <c r="D57" s="58" t="s">
+      <c r="C57" s="54"/>
+      <c r="D57" s="56" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="2:5" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B58" s="60" t="str">
+    <row r="58" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B58" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B52) &lt;= 60,
   "  •  " &amp; _carb_only!B52,
@@ -4066,13 +4047,13 @@
 )</f>
         <v xml:space="preserve">  •  Solid/dry scrape manure collection</v>
       </c>
-      <c r="C58" s="61"/>
-      <c r="D58" s="28" t="s">
+      <c r="C58" s="59"/>
+      <c r="D58" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="2:5" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B59" s="60" t="str">
+    <row r="59" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B59" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B53) &lt;= 60,
   "  •  " &amp; _carb_only!B53,
@@ -4084,13 +4065,13 @@
 )</f>
         <v xml:space="preserve">  •  Vacuum manure collection</v>
       </c>
-      <c r="C59" s="61"/>
-      <c r="D59" s="28" t="s">
+      <c r="C59" s="59"/>
+      <c r="D59" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="2:5" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B60" s="60" t="str">
+    <row r="60" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B60" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B54) &lt;= 60,
   "  •  " &amp; _carb_only!B54,
@@ -4102,13 +4083,13 @@
 )</f>
         <v xml:space="preserve">  •  Liquid/flush manure collection</v>
       </c>
-      <c r="C60" s="61"/>
-      <c r="D60" s="28" t="s">
+      <c r="C60" s="59"/>
+      <c r="D60" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="2:5" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B61" s="60" t="str">
+    <row r="61" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B61" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B55) &lt;= 60,
   "  •  " &amp; _carb_only!B55,
@@ -4120,13 +4101,13 @@
 )</f>
         <v xml:space="preserve">  •  Pasture</v>
       </c>
-      <c r="C61" s="61"/>
-      <c r="D61" s="28" t="s">
+      <c r="C61" s="59"/>
+      <c r="D61" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="2:5" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B62" s="60" t="str">
+    <row r="62" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B62" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B56) &lt;= 60,
   "  •  " &amp; _carb_only!B56,
@@ -4138,13 +4119,13 @@
 )</f>
         <v xml:space="preserve">  •  Dry lot/corral</v>
       </c>
-      <c r="C62" s="61"/>
-      <c r="D62" s="28" t="s">
+      <c r="C62" s="59"/>
+      <c r="D62" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="2:5" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B63" s="60" t="str">
+    <row r="63" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B63" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B57) &lt;= 60,
   "  •  " &amp; _carb_only!B57,
@@ -4156,11 +4137,11 @@
 )</f>
         <v xml:space="preserve">  •  Solid storage</v>
       </c>
-      <c r="C63" s="61"/>
-      <c r="D63" s="28"/>
-    </row>
-    <row r="64" spans="2:5" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B64" s="60" t="str">
+      <c r="C63" s="59"/>
+      <c r="D63" s="27"/>
+    </row>
+    <row r="64" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B64" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B58) &lt;= 60,
   "  •  " &amp; _carb_only!B58,
@@ -4172,13 +4153,13 @@
 )</f>
         <v xml:space="preserve">  •  Solar drying</v>
       </c>
-      <c r="C64" s="61"/>
-      <c r="D64" s="28" t="s">
+      <c r="C64" s="59"/>
+      <c r="D64" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B65" s="60" t="str">
+    <row r="65" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B65" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B59) &lt;= 60,
   "  •  " &amp; _carb_only!B59,
@@ -4190,13 +4171,13 @@
 )</f>
         <v xml:space="preserve">  •  Composting (aerated, in vessel, windrows)</v>
       </c>
-      <c r="C65" s="61"/>
-      <c r="D65" s="28" t="s">
+      <c r="C65" s="59"/>
+      <c r="D65" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B66" s="60" t="str">
+    <row r="66" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B66" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B60) &lt;= 60,
   "  •  " &amp; _carb_only!B60,
@@ -4208,13 +4189,13 @@
 )</f>
         <v xml:space="preserve">  •  Compost bedded pack barn</v>
       </c>
-      <c r="C66" s="61"/>
-      <c r="D66" s="28" t="s">
+      <c r="C66" s="59"/>
+      <c r="D66" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B67" s="60" t="str">
+    <row r="67" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B67" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B61) &lt;= 60,
   "  •  " &amp; _carb_only!B61,
@@ -4226,13 +4207,13 @@
 )</f>
         <v xml:space="preserve">  •  Slatted floor pit storage</v>
       </c>
-      <c r="C67" s="61"/>
-      <c r="D67" s="28" t="s">
+      <c r="C67" s="59"/>
+      <c r="D67" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B68" s="60" t="str">
+    <row r="68" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B68" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B62) &lt;= 60,
   "  •  " &amp; _carb_only!B62,
@@ -4244,13 +4225,13 @@
 )</f>
         <v xml:space="preserve">  •  Anaerobic Lagoon</v>
       </c>
-      <c r="C68" s="61"/>
-      <c r="D68" s="28" t="s">
+      <c r="C68" s="59"/>
+      <c r="D68" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="69" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B69" s="60" t="str">
+    <row r="69" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B69" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B63) &lt;= 60,
   "  •  " &amp; _carb_only!B63,
@@ -4262,13 +4243,13 @@
 )</f>
         <v xml:space="preserve">  •  Anaerobic digester</v>
       </c>
-      <c r="C69" s="61"/>
-      <c r="D69" s="28" t="s">
+      <c r="C69" s="59"/>
+      <c r="D69" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="70" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B70" s="60" t="str">
+    <row r="70" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B70" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B64) &lt;= 60,
   "  •  " &amp; _carb_only!B64,
@@ -4280,13 +4261,13 @@
 )</f>
         <v xml:space="preserve">  •  Vermifiltration</v>
       </c>
-      <c r="C70" s="61"/>
-      <c r="D70" s="28" t="s">
+      <c r="C70" s="59"/>
+      <c r="D70" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B71" s="60" t="str">
+    <row r="71" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B71" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B65) &lt;= 60,
   "  •  " &amp; _carb_only!B65,
@@ -4298,13 +4279,13 @@
 )</f>
         <v xml:space="preserve">  •  Liquid/slurry</v>
       </c>
-      <c r="C71" s="61"/>
-      <c r="D71" s="28" t="s">
+      <c r="C71" s="59"/>
+      <c r="D71" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B72" s="60" t="str">
+    <row r="72" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B72" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B66) &lt;= 60,
   "  •  " &amp; _carb_only!B66,
@@ -4316,13 +4297,13 @@
 )</f>
         <v xml:space="preserve">  •  Mechanical separator (screens, centrifuge, press)</v>
       </c>
-      <c r="C72" s="61"/>
-      <c r="D72" s="28" t="s">
+      <c r="C72" s="59"/>
+      <c r="D72" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="73" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B73" s="60" t="str">
+    <row r="73" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B73" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B67) &lt;= 60,
   "  •  " &amp; _carb_only!B67,
@@ -4334,13 +4315,13 @@
 )</f>
         <v xml:space="preserve">  •  Gravity-based separator (settling basin, sand lane)</v>
       </c>
-      <c r="C73" s="61"/>
-      <c r="D73" s="28" t="s">
+      <c r="C73" s="59"/>
+      <c r="D73" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B74" s="60" t="str">
+    <row r="74" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B74" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B68) &lt;= 60,
   "  •  " &amp; _carb_only!B68,
@@ -4352,13 +4333,13 @@
 )</f>
         <v xml:space="preserve">  •  Weeping wall</v>
       </c>
-      <c r="C74" s="61"/>
-      <c r="D74" s="28" t="s">
+      <c r="C74" s="59"/>
+      <c r="D74" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="75" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B75" s="60" t="str">
+    <row r="75" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B75" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B69) &lt;= 60,
   "  •  " &amp; _carb_only!B69,
@@ -4370,13 +4351,13 @@
 )</f>
         <v xml:space="preserve">  •  Flocculation</v>
       </c>
-      <c r="C75" s="61"/>
-      <c r="D75" s="28" t="s">
+      <c r="C75" s="59"/>
+      <c r="D75" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="76" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B76" s="60" t="str">
+    <row r="76" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B76" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B70) &lt;= 60,
   "  •  " &amp; _carb_only!B70,
@@ -4388,13 +4369,13 @@
 )</f>
         <v xml:space="preserve">  •  Daily spread</v>
       </c>
-      <c r="C76" s="61"/>
-      <c r="D76" s="28" t="s">
+      <c r="C76" s="59"/>
+      <c r="D76" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="77" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B77" s="60" t="str">
+    <row r="77" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B77" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B71) &lt;= 60,
   "  •  " &amp; _carb_only!B71,
@@ -4406,13 +4387,13 @@
 )</f>
         <v xml:space="preserve">  •  Land application (flood)</v>
       </c>
-      <c r="C77" s="61"/>
-      <c r="D77" s="28" t="s">
+      <c r="C77" s="59"/>
+      <c r="D77" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="78" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B78" s="60" t="str">
+    <row r="78" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B78" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B72) &lt;= 60,
   "  •  " &amp; _carb_only!B72,
@@ -4424,22 +4405,22 @@
 )</f>
         <v xml:space="preserve">  •  Land application (subsurface drip)</v>
       </c>
-      <c r="C78" s="61"/>
-      <c r="D78" s="28" t="s">
+      <c r="C78" s="59"/>
+      <c r="D78" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="79" spans="2:7" s="52" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B79" s="58" t="s">
+    <row r="79" spans="2:7" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B79" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="C79" s="56"/>
-      <c r="D79" s="58" t="s">
+      <c r="C79" s="54"/>
+      <c r="D79" s="56" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="80" spans="2:7" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.5">
-      <c r="B80" s="60" t="str">
+    <row r="80" spans="2:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.5">
+      <c r="B80" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B76) &lt;= 60,
   "  •  " &amp; _carb_only!B76,
@@ -4452,14 +4433,14 @@
         <v xml:space="preserve">  •  Biogas conditioning (e.g., hydrogen sulfide, moisture,
      particulate removal)</v>
       </c>
-      <c r="C80" s="61"/>
-      <c r="D80" s="28" t="s">
+      <c r="C80" s="59"/>
+      <c r="D80" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G80" s="62"/>
-    </row>
-    <row r="81" spans="2:7" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.5">
-      <c r="B81" s="60" t="str">
+      <c r="G80"/>
+    </row>
+    <row r="81" spans="2:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.5">
+      <c r="B81" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B77) &lt;= 60,
   "  •  " &amp; _carb_only!B77,
@@ -4472,14 +4453,14 @@
         <v xml:space="preserve">  •  Biogas moving and handling equipement (e.g., blower,
      compressor, low pressure gas pipelines)</v>
       </c>
-      <c r="C81" s="61"/>
-      <c r="D81" s="28" t="s">
+      <c r="C81" s="59"/>
+      <c r="D81" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G81" s="62"/>
-    </row>
-    <row r="82" spans="2:7" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.5">
-      <c r="B82" s="60" t="str">
+      <c r="G81"/>
+    </row>
+    <row r="82" spans="2:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.5">
+      <c r="B82" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B78) &lt;= 60,
   "  •  " &amp; _carb_only!B78,
@@ -4492,14 +4473,14 @@
         <v xml:space="preserve">  •  Biomethane upgrading (e.g., membrane or other form of CO2
      removal)</v>
       </c>
-      <c r="C82" s="61"/>
-      <c r="D82" s="28" t="s">
+      <c r="C82" s="59"/>
+      <c r="D82" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G82" s="62"/>
-    </row>
-    <row r="83" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B83" s="60" t="str">
+      <c r="G82"/>
+    </row>
+    <row r="83" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B83" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B79) &lt;= 60,
   "  •  " &amp; _carb_only!B79,
@@ -4511,14 +4492,14 @@
 )</f>
         <v xml:space="preserve">  •  Covered lagoon anaerobic digester</v>
       </c>
-      <c r="C83" s="61"/>
-      <c r="D83" s="28" t="s">
+      <c r="C83" s="59"/>
+      <c r="D83" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G83" s="62"/>
-    </row>
-    <row r="84" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B84" s="60" t="str">
+      <c r="G83"/>
+    </row>
+    <row r="84" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B84" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B80) &lt;= 60,
   "  •  " &amp; _carb_only!B80,
@@ -4530,14 +4511,14 @@
 )</f>
         <v xml:space="preserve">  •  In-vessel anaerobic digester</v>
       </c>
-      <c r="C84" s="61"/>
-      <c r="D84" s="28" t="s">
+      <c r="C84" s="59"/>
+      <c r="D84" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G84" s="62"/>
-    </row>
-    <row r="85" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B85" s="60" t="str">
+      <c r="G84"/>
+    </row>
+    <row r="85" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B85" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B81) &lt;= 60,
   "  •  " &amp; _carb_only!B81,
@@ -4549,14 +4530,14 @@
 )</f>
         <v xml:space="preserve">  •  Electricity generation or other combustion equipment</v>
       </c>
-      <c r="C85" s="61"/>
-      <c r="D85" s="28" t="s">
+      <c r="C85" s="59"/>
+      <c r="D85" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G85" s="62"/>
-    </row>
-    <row r="86" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B86" s="60" t="str">
+      <c r="G85"/>
+    </row>
+    <row r="86" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B86" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B82) &lt;= 60,
   "  •  " &amp; _carb_only!B82,
@@ -4568,14 +4549,14 @@
 )</f>
         <v xml:space="preserve">  •  Heating/process fuel equipment</v>
       </c>
-      <c r="C86" s="61"/>
-      <c r="D86" s="28" t="s">
+      <c r="C86" s="59"/>
+      <c r="D86" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G86" s="62"/>
-    </row>
-    <row r="87" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B87" s="60" t="str">
+      <c r="G86"/>
+    </row>
+    <row r="87" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B87" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B83) &lt;= 60,
   "  •  " &amp; _carb_only!B83,
@@ -4587,14 +4568,14 @@
 )</f>
         <v xml:space="preserve">  •  Fuel cells</v>
       </c>
-      <c r="C87" s="61"/>
-      <c r="D87" s="28" t="s">
+      <c r="C87" s="59"/>
+      <c r="D87" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G87" s="62"/>
-    </row>
-    <row r="88" spans="2:7" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.5">
-      <c r="B88" s="60" t="str">
+      <c r="G87"/>
+    </row>
+    <row r="88" spans="2:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.5">
+      <c r="B88" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B84) &lt;= 60,
   "  •  " &amp; _carb_only!B84,
@@ -4607,14 +4588,14 @@
         <v xml:space="preserve">  •  Common carrier gas pipeline (Interconnection point of
      receipt)</v>
       </c>
-      <c r="C88" s="61"/>
-      <c r="D88" s="28" t="s">
+      <c r="C88" s="59"/>
+      <c r="D88" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G88" s="62"/>
-    </row>
-    <row r="89" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B89" s="60" t="str">
+      <c r="G88"/>
+    </row>
+    <row r="89" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B89" s="58" t="str">
         <f>IF(
   LEN(_carb_only!B85) &lt;= 60,
   "  •  " &amp; _carb_only!B85,
@@ -4626,56 +4607,56 @@
 )</f>
         <v xml:space="preserve">  •  Onsite fuel use or dispensing</v>
       </c>
-      <c r="C89" s="61"/>
-      <c r="D89" s="28" t="s">
+      <c r="C89" s="59"/>
+      <c r="D89" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G89" s="62"/>
-    </row>
-    <row r="90" spans="2:7" s="52" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="B90" s="58" t="s">
+      <c r="G89"/>
+    </row>
+    <row r="90" spans="2:7" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+      <c r="B90" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="D90" s="30" t="s">
+      <c r="D90" s="29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="91" spans="2:7" s="52" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
-      <c r="B91" s="58" t="s">
+    <row r="91" spans="2:7" s="10" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
+      <c r="B91" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="D91" s="30" t="s">
+      <c r="D91" s="29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="92" spans="2:7" s="52" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
-      <c r="B92" s="58" t="s">
+    <row r="92" spans="2:7" s="10" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
+      <c r="B92" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="D92" s="30" t="s">
+      <c r="D92" s="29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="93" spans="2:7" s="52" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
-      <c r="B93" s="58" t="s">
+    <row r="93" spans="2:7" s="10" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
+      <c r="B93" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="D93" s="30" t="s">
+      <c r="D93" s="29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="94" spans="2:7" s="52" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B94" s="56"/>
-      <c r="D94" s="63"/>
-    </row>
-    <row r="95" spans="2:7" s="64" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="96" spans="2:7" s="64" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="97" spans="2:4" s="52" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
-      <c r="B97" s="58" t="s">
+    <row r="94" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+      <c r="B94" s="54"/>
+      <c r="D94" s="60"/>
+    </row>
+    <row r="95" spans="2:7" s="17" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="96" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="97" spans="2:4" s="10" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
+      <c r="B97" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C97" s="65"/>
-      <c r="D97" s="30" t="s">
+      <c r="C97" s="61"/>
+      <c r="D97" s="29" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4786,7 +4767,7 @@
       <c r="B12" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="28">
         <v>45819</v>
       </c>
       <c r="D12" s="13" t="s">
@@ -4797,7 +4778,7 @@
       <c r="B13" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="28">
         <v>45838</v>
       </c>
       <c r="D13" s="13" t="s">
@@ -4817,7 +4798,7 @@
       <c r="B15" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="28">
         <v>45841</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -4828,7 +4809,7 @@
       <c r="B16" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="29">
+      <c r="C16" s="28">
         <v>45846</v>
       </c>
       <c r="D16" s="13" t="s">
@@ -5046,7 +5027,7 @@
       <c r="B19" s="10">
         <v>1</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="22" t="s">
         <v>93</v>
       </c>
       <c r="D19" s="14">
@@ -5106,7 +5087,7 @@
       <c r="B22" s="10">
         <v>4</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="25" t="s">
         <v>101</v>
       </c>
       <c r="D22" s="14">
@@ -5118,7 +5099,7 @@
       <c r="F22" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G22" s="27" t="s">
+      <c r="G22" s="26" t="s">
         <v>103</v>
       </c>
     </row>
@@ -5200,7 +5181,7 @@
       <c r="B27" s="10">
         <v>9</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="25" t="s">
         <v>110</v>
       </c>
       <c r="D27" s="14">
@@ -5240,7 +5221,7 @@
       <c r="B29" s="10">
         <v>11</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="19" t="s">
         <v>114</v>
       </c>
       <c r="D29" s="14">
@@ -5255,7 +5236,7 @@
       <c r="B30" s="10">
         <v>12</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="19" t="s">
         <v>115</v>
       </c>
       <c r="D30" s="14">
@@ -5781,15 +5762,15 @@
       <c r="F83" s="13"/>
       <c r="G83" s="13"/>
     </row>
-    <row r="84" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="84" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B84" s="10">
         <v>66</v>
       </c>
-      <c r="C84" s="24"/>
-      <c r="D84" s="25"/>
+      <c r="C84" s="23"/>
+      <c r="D84" s="24"/>
       <c r="E84" s="10"/>
       <c r="F84" s="13"/>
-      <c r="G84" s="24"/>
+      <c r="G84" s="23"/>
     </row>
     <row r="85" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B85" s="10">
@@ -5805,7 +5786,7 @@
         <v>68</v>
       </c>
       <c r="C86" s="13"/>
-      <c r="D86" s="25"/>
+      <c r="D86" s="24"/>
       <c r="F86" s="13"/>
       <c r="G86" s="13"/>
     </row>
@@ -5825,7 +5806,7 @@
       <c r="C88" s="13"/>
       <c r="D88" s="14"/>
       <c r="F88" s="13"/>
-      <c r="G88" s="20"/>
+      <c r="G88" s="19"/>
     </row>
     <row r="89" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B89" s="10">
@@ -5834,7 +5815,7 @@
       <c r="C89" s="13"/>
       <c r="D89" s="14"/>
       <c r="F89" s="13"/>
-      <c r="G89" s="20"/>
+      <c r="G89" s="19"/>
     </row>
     <row r="90" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B90" s="10">
@@ -5852,13 +5833,13 @@
       <c r="C91" s="13"/>
       <c r="D91" s="14"/>
       <c r="F91" s="13"/>
-      <c r="G91" s="20"/>
+      <c r="G91" s="19"/>
     </row>
     <row r="92" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B92" s="10">
         <v>74</v>
       </c>
-      <c r="C92" s="21"/>
+      <c r="C92" s="20"/>
       <c r="D92" s="14"/>
       <c r="F92" s="13"/>
       <c r="G92" s="13"/>
@@ -5971,7 +5952,7 @@
       <c r="F104" s="13"/>
       <c r="G104" s="13"/>
     </row>
-    <row r="105" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="105" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B105" s="10">
         <v>87</v>
       </c>
@@ -5981,7 +5962,7 @@
       <c r="F105" s="13"/>
       <c r="G105" s="13"/>
     </row>
-    <row r="106" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="106" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B106" s="10">
         <v>88</v>
       </c>
@@ -5991,7 +5972,7 @@
       <c r="F106" s="13"/>
       <c r="G106" s="13"/>
     </row>
-    <row r="107" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="107" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B107" s="10">
         <v>89</v>
       </c>
@@ -6001,7 +5982,7 @@
       <c r="F107" s="13"/>
       <c r="G107" s="13"/>
     </row>
-    <row r="108" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="108" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B108" s="10">
         <v>90</v>
       </c>
@@ -6011,7 +5992,7 @@
       <c r="F108" s="13"/>
       <c r="G108" s="13"/>
     </row>
-    <row r="109" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="109" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B109" s="10">
         <v>91</v>
       </c>
@@ -6021,7 +6002,7 @@
       <c r="F109" s="13"/>
       <c r="G109" s="13"/>
     </row>
-    <row r="110" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="110" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B110" s="10">
         <v>92</v>
       </c>
@@ -6040,7 +6021,7 @@
       <c r="F111" s="13"/>
       <c r="G111" s="13"/>
     </row>
-    <row r="112" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="112" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B112" s="10">
         <v>94</v>
       </c>
@@ -6050,7 +6031,7 @@
       <c r="F112" s="13"/>
       <c r="G112" s="13"/>
     </row>
-    <row r="113" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="113" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B113" s="10">
         <v>95</v>
       </c>
@@ -6060,7 +6041,7 @@
       <c r="F113" s="13"/>
       <c r="G113" s="13"/>
     </row>
-    <row r="114" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="114" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B114" s="10">
         <v>96</v>
       </c>
@@ -6070,7 +6051,7 @@
       <c r="F114" s="13"/>
       <c r="G114" s="13"/>
     </row>
-    <row r="115" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="115" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B115" s="10">
         <v>97</v>
       </c>
@@ -6080,7 +6061,7 @@
       <c r="F115" s="13"/>
       <c r="G115" s="13"/>
     </row>
-    <row r="116" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="116" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B116" s="10">
         <v>98</v>
       </c>
@@ -6090,7 +6071,7 @@
       <c r="F116" s="13"/>
       <c r="G116" s="13"/>
     </row>
-    <row r="117" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="117" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B117" s="10">
         <v>99</v>
       </c>
@@ -6100,7 +6081,7 @@
       <c r="F117" s="13"/>
       <c r="G117" s="13"/>
     </row>
-    <row r="118" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="118" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B118" s="10">
         <v>100</v>
       </c>
@@ -6228,8 +6209,8 @@
       <c r="P7"/>
       <c r="Q7"/>
     </row>
-    <row r="10" spans="1:17" s="22" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
-      <c r="B10" s="22" t="s">
+    <row r="10" spans="1:17" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B10" s="21" t="s">
         <v>126</v>
       </c>
       <c r="D10"/>
@@ -6843,8 +6824,8 @@
     <row r="87" spans="2:17" x14ac:dyDescent="0.5">
       <c r="G87"/>
     </row>
-    <row r="88" spans="2:17" s="22" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
-      <c r="B88" s="22" t="s">
+    <row r="88" spans="2:17" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B88" s="21" t="s">
         <v>187</v>
       </c>
       <c r="D88"/>
@@ -6920,8 +6901,8 @@
       <c r="F98"/>
       <c r="Q98"/>
     </row>
-    <row r="99" spans="2:17" s="22" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
-      <c r="B99" s="22" t="s">
+    <row r="99" spans="2:17" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B99" s="21" t="s">
         <v>189</v>
       </c>
       <c r="D99"/>
@@ -7011,8 +6992,8 @@
         <v>Stacking slab/stockpile/other manure storage</v>
       </c>
     </row>
-    <row r="118" spans="2:17" s="22" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
-      <c r="B118" s="22" t="s">
+    <row r="118" spans="2:17" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B118" s="21" t="s">
         <v>190</v>
       </c>
       <c r="D118"/>
@@ -7077,8 +7058,8 @@
         <v>Venting-intentional/routine</v>
       </c>
     </row>
-    <row r="132" spans="2:17" s="22" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
-      <c r="B132" s="22" t="s">
+    <row r="132" spans="2:17" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B132" s="21" t="s">
         <v>191</v>
       </c>
       <c r="D132"/>
@@ -7118,8 +7099,8 @@
         <v>No</v>
       </c>
     </row>
-    <row r="141" spans="2:17" s="22" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
-      <c r="B141" s="22" t="s">
+    <row r="141" spans="2:17" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B141" s="21" t="s">
         <v>192</v>
       </c>
       <c r="D141"/>
@@ -7317,8 +7298,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="2:17" s="22" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
-      <c r="B180" s="22" t="s">
+    <row r="180" spans="2:17" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B180" s="21" t="s">
         <v>193</v>
       </c>
       <c r="D180"/>
@@ -7616,7 +7597,7 @@
   <dimension ref="A2:F71"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A11" sqref="A11:F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -7908,7 +7889,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>249</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.5">
@@ -7916,16 +7897,16 @@
         <v>201</v>
       </c>
       <c r="C27" t="s">
+        <v>249</v>
+      </c>
+      <c r="D27" t="s">
         <v>250</v>
-      </c>
-      <c r="D27" t="s">
-        <v>251</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>252</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.5">
@@ -7933,10 +7914,10 @@
         <v>201</v>
       </c>
       <c r="C28" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D28" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -7950,10 +7931,10 @@
         <v>201</v>
       </c>
       <c r="C29" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D29" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -7967,10 +7948,10 @@
         <v>201</v>
       </c>
       <c r="C30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E30" t="b">
         <v>1</v>
@@ -7984,10 +7965,10 @@
         <v>201</v>
       </c>
       <c r="C31" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D31" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>
@@ -7998,10 +7979,10 @@
         <v>201</v>
       </c>
       <c r="C32" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D32" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E32" t="b">
         <v>1</v>
@@ -8015,10 +7996,10 @@
         <v>201</v>
       </c>
       <c r="C33" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D33" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -8029,10 +8010,10 @@
         <v>201</v>
       </c>
       <c r="C34" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D34" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E34" t="b">
         <v>1</v>
@@ -8046,10 +8027,10 @@
         <v>201</v>
       </c>
       <c r="C35" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D35" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
@@ -8063,10 +8044,10 @@
         <v>201</v>
       </c>
       <c r="C36" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D36" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -8080,10 +8061,10 @@
         <v>201</v>
       </c>
       <c r="C37" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D37" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -8097,16 +8078,16 @@
         <v>201</v>
       </c>
       <c r="C38" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D38" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
       </c>
       <c r="F38">
-        <v>447</v>
+        <v>7143</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.5">
@@ -8114,10 +8095,10 @@
         <v>201</v>
       </c>
       <c r="C39" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D39" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
@@ -8128,10 +8109,10 @@
         <v>201</v>
       </c>
       <c r="C40" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D40" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E40" t="b">
         <v>0</v>
@@ -8142,10 +8123,10 @@
         <v>201</v>
       </c>
       <c r="C41" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D41" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E41" t="b">
         <v>0</v>
@@ -8156,16 +8137,16 @@
         <v>201</v>
       </c>
       <c r="C42" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D42" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>35.321100000000001</v>
+        <v>36.076599999999999</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.5">
@@ -8173,10 +8154,10 @@
         <v>201</v>
       </c>
       <c r="C43" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D43" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -8190,16 +8171,16 @@
         <v>201</v>
       </c>
       <c r="C44" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D44" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
       </c>
       <c r="F44">
-        <v>-119.5808</v>
+        <v>-119.44289999999999</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.5">
@@ -8207,10 +8188,10 @@
         <v>201</v>
       </c>
       <c r="C45" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D45" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E45" t="b">
         <v>0</v>
@@ -8221,16 +8202,13 @@
         <v>201</v>
       </c>
       <c r="C46" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D46" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
-      </c>
-      <c r="F46" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.5">
@@ -8238,10 +8216,10 @@
         <v>201</v>
       </c>
       <c r="C47" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D47" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
@@ -8252,246 +8230,234 @@
         <v>201</v>
       </c>
       <c r="C48" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D48" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B49" t="s">
         <v>201</v>
       </c>
       <c r="C49" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D49" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B50" t="s">
         <v>201</v>
       </c>
       <c r="C50" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D50" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B51" t="s">
         <v>201</v>
       </c>
       <c r="C51" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D51" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B52" t="s">
         <v>201</v>
       </c>
       <c r="C52" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D52" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E52" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B53" t="s">
         <v>201</v>
       </c>
       <c r="C53" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D53" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E53" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B54" t="s">
         <v>201</v>
       </c>
       <c r="C54" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D54" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E54" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B55" t="s">
         <v>201</v>
       </c>
       <c r="C55" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D55" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E55" t="b">
         <v>0</v>
       </c>
-      <c r="F55" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.5">
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B56" t="s">
         <v>201</v>
       </c>
       <c r="C56" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D56" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E56" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B57" t="s">
         <v>201</v>
       </c>
       <c r="C57" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D57" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E57" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B58" t="s">
         <v>201</v>
       </c>
       <c r="C58" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D58" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E58" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B59" t="s">
         <v>201</v>
       </c>
       <c r="C59" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D59" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E59" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B60" t="s">
         <v>201</v>
       </c>
       <c r="C60" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D60" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E60" t="b">
         <v>0</v>
       </c>
-      <c r="F60" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.5">
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B61" t="s">
         <v>201</v>
       </c>
       <c r="C61" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D61" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E61" t="b">
         <v>0</v>
       </c>
-      <c r="F61" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.5">
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B62" t="s">
         <v>201</v>
       </c>
       <c r="C62" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D62" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E62" t="b">
         <v>0</v>
       </c>
-      <c r="F62" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.5">
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B63" t="s">
         <v>201</v>
       </c>
       <c r="C63" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D63" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E63" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B64" t="s">
         <v>201</v>
       </c>
       <c r="C64" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D64" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E64" t="b">
         <v>0</v>
@@ -8502,10 +8468,10 @@
         <v>201</v>
       </c>
       <c r="C65" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D65" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E65" t="b">
         <v>0</v>
@@ -8516,10 +8482,10 @@
         <v>201</v>
       </c>
       <c r="C66" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D66" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="E66" t="b">
         <v>0</v>
@@ -8530,10 +8496,10 @@
         <v>201</v>
       </c>
       <c r="C67" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D67" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E67" t="b">
         <v>0</v>
@@ -8544,16 +8510,16 @@
         <v>201</v>
       </c>
       <c r="C68" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D68" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E68" t="b">
         <v>0</v>
       </c>
-      <c r="F68" s="17">
-        <v>45468</v>
+      <c r="F68" s="62">
+        <v>45782.517916666664</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.5">
@@ -8561,10 +8527,10 @@
         <v>201</v>
       </c>
       <c r="C69" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D69" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E69" t="b">
         <v>0</v>
@@ -8575,10 +8541,10 @@
         <v>201</v>
       </c>
       <c r="C70" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D70" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E70" t="b">
         <v>0</v>
@@ -8589,10 +8555,10 @@
         <v>201</v>
       </c>
       <c r="C71" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D71" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E71" t="b">
         <v>0</v>

</xml_diff>